<commit_message>
Finalized mesh_constraints transfer. Some xlsx's still not working
</commit_message>
<xml_diff>
--- a/Testing/data/optimize/mesh_constraints/optimize.xlsx
+++ b/Testing/data/optimize/mesh_constraints/optimize.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="193">
   <si>
     <t>shape_1</t>
   </si>
@@ -565,6 +565,45 @@
   </si>
   <si>
     <t>zoom_state</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere10_groomed_local.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere10_groomed_world.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere20_groomed_local.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere20_groomed_world.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere30_groomed_local.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere30_groomed_world.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere40_groomed_local.particles</t>
+  </si>
+  <si>
+    <t>/home/hxu/Documents/ShapeWorks/Testing/data/optimize/mesh_constraints/optimize_particles/sphere40_groomed_world.particles</t>
+  </si>
+  <si>
+    <t>0.500000</t>
+  </si>
+  <si>
+    <t>15.000000</t>
+  </si>
+  <si>
+    <t>1000.000000</t>
+  </si>
+  <si>
+    <t>5.000000</t>
+  </si>
+  <si>
+    <t>100.000000</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1126,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1103,7 +1142,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1610,7 +1649,7 @@
         <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1618,7 +1657,7 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Removed all optimize tests
</commit_message>
<xml_diff>
--- a/Testing/data/optimize/mesh_constraints/optimize.xlsx
+++ b/Testing/data/optimize/mesh_constraints/optimize.xlsx
@@ -12,16 +12,16 @@
     <sheet name="groom" sheetId="3" r:id="rId3"/>
     <sheet name="studio" sheetId="4" r:id="rId4"/>
     <sheet name="project" sheetId="5" r:id="rId5"/>
-    <sheet name="landmarks" sheetId="6" r:id="rId6"/>
-    <sheet name="analysis" sheetId="7" r:id="rId7"/>
-    <sheet name="deepssm" sheetId="8" r:id="rId8"/>
+    <sheet name="analysis" sheetId="7" r:id="rId6"/>
+    <sheet name="deepssm" sheetId="8" r:id="rId7"/>
+    <sheet name="landmarks" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="194">
   <si>
     <t>shape_1</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>100.000000</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1134,7 +1137,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1649,7 +1652,7 @@
         <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1657,7 +1660,7 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1713,32 +1716,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
@@ -1899,4 +1876,30 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>